<commit_message>
draft version of execution graph and basic interfaces for that graph to work
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-core/src/main/resources/excel/1.xlsx
+++ b/calculation-engine/engine-core/src/main/resources/excel/1.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="2355" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="3255" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -350,121 +350,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
-        <f>B1+B2</f>
-        <v>11.333333333333334</v>
+        <f>5-IF(I1=I2,I3,I4)</f>
+        <v>1</v>
       </c>
       <c r="B1">
-        <f>C1</f>
-        <v>5.666666666666667</v>
-      </c>
-      <c r="C1">
-        <f>D1+E1</f>
-        <v>5.666666666666667</v>
-      </c>
-      <c r="D1">
-        <f>D3</f>
+        <v>10</v>
+      </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f>D9</f>
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f>B5+B5</f>
         <v>4</v>
       </c>
-      <c r="E1">
-        <f>E3</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="F1">
-        <f>B6-B7</f>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f>D5-E5</f>
+        <v>2</v>
+      </c>
+      <c r="D5">
         <v>5</v>
       </c>
-      <c r="G1">
-        <f>A6-A7</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <f>C2</f>
-        <v>5.666666666666667</v>
-      </c>
-      <c r="C2">
-        <f>D2+E2</f>
-        <v>5.666666666666667</v>
-      </c>
-      <c r="D2">
-        <f>D3</f>
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <f>E3</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="F2">
-        <v>6</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D3">
-        <f>F4*G4</f>
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <f>F4*F5</f>
-        <v>1.6666666666666667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <f>G1/G2</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F5">
-        <f>F1/F2</f>
-        <v>0.83333333333333337</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>12</v>
-      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <f>IF(C7=56,B8,B9)</f>
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f>COUNT(D1:D8)</f>
         <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>